<commit_message>
Code for journal article
</commit_message>
<xml_diff>
--- a/Table_S1.xlsx
+++ b/Table_S1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzopellis/Desktop/GrowthDelay_all_versions/Growth rate paper PhilTransB/GrowthDelayCodes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0807855E-1EBF-FE45-B944-E884A1E4AAE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290DE5DD-BD33-1946-8FBC-597DBA0F0E95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prodrmal period" sheetId="2" r:id="rId1"/>
@@ -136,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -191,7 +191,55 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -204,58 +252,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
@@ -265,19 +265,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -295,32 +282,6 @@
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
@@ -386,17 +347,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -422,48 +372,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -496,6 +404,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -562,7 +528,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -570,68 +536,59 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1035,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1045,46 +1002,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="30" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="30" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="36"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="1">
         <v>0</v>
       </c>
@@ -1103,245 +1060,245 @@
       <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="4">
         <v>2</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+      <c r="A4" s="5">
         <v>0.1</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="6">
         <v>6.9314718055994504</v>
       </c>
-      <c r="C4" s="12">
-        <v>1.8820060258390101</v>
-      </c>
-      <c r="D4" s="13">
-        <v>1.7041321038544099</v>
-      </c>
-      <c r="E4" s="13">
-        <v>1.54629188736362</v>
-      </c>
-      <c r="F4" s="14">
-        <v>1.39883076741894</v>
-      </c>
-      <c r="G4" s="12">
-        <v>2.0325735957841302</v>
-      </c>
-      <c r="H4" s="13">
-        <v>1.84005152185302</v>
-      </c>
-      <c r="I4" s="15">
-        <v>1.6626998842258001</v>
-      </c>
-      <c r="J4" s="11">
-        <v>1.5196373859452701</v>
+      <c r="C4" s="23">
+        <v>1.88388863325447</v>
+      </c>
+      <c r="D4" s="24">
+        <v>1.70585322928297</v>
+      </c>
+      <c r="E4" s="24">
+        <v>1.54766029450716</v>
+      </c>
+      <c r="F4" s="25">
+        <v>1.4002636072850501</v>
+      </c>
+      <c r="G4" s="22">
+        <v>2.0345386714793801</v>
+      </c>
+      <c r="H4" s="24">
+        <v>1.8421219476233901</v>
+      </c>
+      <c r="I4" s="24">
+        <v>1.6642387265652101</v>
+      </c>
+      <c r="J4" s="25">
+        <v>1.5211149914836299</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
+      <c r="A5" s="7">
         <v>0.15</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="8">
         <v>4.6209812037329696</v>
       </c>
-      <c r="C5" s="18">
-        <v>2.50793331853375</v>
-      </c>
-      <c r="D5" s="19">
-        <v>2.16367177361936</v>
-      </c>
-      <c r="E5" s="19">
-        <v>1.8728334254083101</v>
-      </c>
-      <c r="F5" s="20">
-        <v>1.6179183263067101</v>
-      </c>
-      <c r="G5" s="18">
-        <v>2.8087057864516298</v>
-      </c>
-      <c r="H5" s="19">
-        <v>2.42291735193669</v>
-      </c>
-      <c r="I5" s="21">
-        <v>2.0863351528868499</v>
-      </c>
-      <c r="J5" s="17">
-        <v>1.8254382677533501</v>
+      <c r="C5" s="23">
+        <v>2.5116776205658602</v>
+      </c>
+      <c r="D5" s="24">
+        <v>2.1669299289289001</v>
+      </c>
+      <c r="E5" s="24">
+        <v>1.87527686810844</v>
+      </c>
+      <c r="F5" s="25">
+        <v>1.6203253580883801</v>
+      </c>
+      <c r="G5" s="22">
+        <v>2.8127475503541701</v>
+      </c>
+      <c r="H5" s="24">
+        <v>2.4269335843042601</v>
+      </c>
+      <c r="I5" s="24">
+        <v>2.0893311393909499</v>
+      </c>
+      <c r="J5" s="25">
+        <v>1.8279844299361501</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+      <c r="A6" s="7">
         <v>0.2</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="8">
         <v>3.4657359027997301</v>
       </c>
-      <c r="C6" s="18">
-        <v>3.2877270280600199</v>
-      </c>
-      <c r="D6" s="19">
-        <v>2.7056285945719898</v>
-      </c>
-      <c r="E6" s="19">
-        <v>2.2374370261733199</v>
-      </c>
-      <c r="F6" s="20">
-        <v>1.85109683254291</v>
-      </c>
-      <c r="G6" s="18">
-        <v>3.8121062677199098</v>
-      </c>
-      <c r="H6" s="19">
-        <v>3.1376248246424199</v>
-      </c>
-      <c r="I6" s="21">
-        <v>2.5795109720060201</v>
-      </c>
-      <c r="J6" s="17">
-        <v>2.1649500385952498</v>
+      <c r="C6" s="23">
+        <v>3.2942278522392199</v>
+      </c>
+      <c r="D6" s="24">
+        <v>2.71101497912248</v>
+      </c>
+      <c r="E6" s="24">
+        <v>2.2412534685446301</v>
+      </c>
+      <c r="F6" s="25">
+        <v>1.8546431169067199</v>
+      </c>
+      <c r="G6" s="22">
+        <v>3.81935214311163</v>
+      </c>
+      <c r="H6" s="24">
+        <v>3.1444291721574902</v>
+      </c>
+      <c r="I6" s="24">
+        <v>2.5845366518663799</v>
+      </c>
+      <c r="J6" s="25">
+        <v>2.1688246178745199</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="16">
+      <c r="A7" s="7">
         <v>0.25</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="8">
         <v>2.7725887222397798</v>
       </c>
-      <c r="C7" s="18">
-        <v>4.24749217574103</v>
-      </c>
-      <c r="D7" s="19">
-        <v>3.33851510255543</v>
-      </c>
-      <c r="E7" s="19">
-        <v>2.6419314525216602</v>
-      </c>
-      <c r="F7" s="20">
-        <v>2.0987565923612999</v>
-      </c>
-      <c r="G7" s="18">
-        <v>5.0908229202040998</v>
-      </c>
-      <c r="H7" s="19">
-        <v>4.0032410315714602</v>
-      </c>
-      <c r="I7" s="21">
-        <v>3.14834431862911</v>
-      </c>
-      <c r="J7" s="17">
-        <v>2.5399404843037701</v>
+      <c r="C7" s="23">
+        <v>4.2579071247868798</v>
+      </c>
+      <c r="D7" s="24">
+        <v>3.3467390210526902</v>
+      </c>
+      <c r="E7" s="24">
+        <v>2.6474475496229699</v>
+      </c>
+      <c r="F7" s="25">
+        <v>2.1036083777657901</v>
+      </c>
+      <c r="G7" s="22">
+        <v>5.1027915403390498</v>
+      </c>
+      <c r="H7" s="24">
+        <v>4.0138864074578198</v>
+      </c>
+      <c r="I7" s="24">
+        <v>3.1560666379429998</v>
+      </c>
+      <c r="J7" s="25">
+        <v>2.5454251012054399</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="22">
+      <c r="A8" s="9">
         <v>0.3</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="10">
         <v>2.3104906018664799</v>
       </c>
-      <c r="C8" s="24">
-        <v>5.4160277204744602</v>
-      </c>
-      <c r="D8" s="25">
-        <v>4.0711810781303903</v>
-      </c>
-      <c r="E8" s="25">
-        <v>3.0881321531897301</v>
-      </c>
-      <c r="F8" s="26">
-        <v>2.3612188693342402</v>
-      </c>
-      <c r="G8" s="24">
-        <v>6.6993738033652903</v>
-      </c>
-      <c r="H8" s="25">
-        <v>5.0400953873580701</v>
-      </c>
-      <c r="I8" s="27">
-        <v>3.79902285679609</v>
-      </c>
-      <c r="J8" s="23">
-        <v>2.9520557811914299</v>
+      <c r="C8" s="23">
+        <v>5.4318235557453702</v>
+      </c>
+      <c r="D8" s="24">
+        <v>4.0830804001140102</v>
+      </c>
+      <c r="E8" s="24">
+        <v>3.0957031746911401</v>
+      </c>
+      <c r="F8" s="25">
+        <v>2.3675449685819201</v>
+      </c>
+      <c r="G8" s="22">
+        <v>6.7180609715133999</v>
+      </c>
+      <c r="H8" s="24">
+        <v>5.05587372087329</v>
+      </c>
+      <c r="I8" s="24">
+        <v>3.8102093821151599</v>
+      </c>
+      <c r="J8" s="25">
+        <v>2.9594538635358401</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="3">
-        <v>6.7621454367849303</v>
-      </c>
-      <c r="D9" s="4">
-        <v>5.7632175688700897</v>
-      </c>
-      <c r="E9" s="4">
-        <v>4.7835433523565696</v>
-      </c>
-      <c r="F9" s="7">
-        <v>3.71575211167037</v>
-      </c>
-      <c r="G9" s="3">
-        <v>7.5630716787236496</v>
-      </c>
-      <c r="H9" s="4">
-        <v>6.5508752375587198</v>
-      </c>
-      <c r="I9" s="9">
-        <v>5.5122400149350703</v>
-      </c>
-      <c r="J9" s="6">
-        <v>4.5879766576935301</v>
+      <c r="B9" s="21"/>
+      <c r="C9" s="26">
+        <v>6.7721691903670997</v>
+      </c>
+      <c r="D9" s="27">
+        <v>5.7733231542130099</v>
+      </c>
+      <c r="E9" s="27">
+        <v>4.7926203916714103</v>
+      </c>
+      <c r="F9" s="28">
+        <v>3.7268778353160901</v>
+      </c>
+      <c r="G9" s="29">
+        <v>7.5728207550845603</v>
+      </c>
+      <c r="H9" s="27">
+        <v>6.5625130003364696</v>
+      </c>
+      <c r="I9" s="27">
+        <v>5.5201336338797198</v>
+      </c>
+      <c r="J9" s="28">
+        <v>4.5980146844562801</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="30" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="32"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="30" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="32"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="1">
         <v>0</v>
       </c>
@@ -1360,212 +1317,205 @@
       <c r="H13" s="2">
         <v>1</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="4">
         <v>2</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
+      <c r="A14" s="5">
         <v>0.1</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="6">
         <v>6.9314718055994504</v>
       </c>
-      <c r="C14" s="12">
-        <v>1.6338421454843</v>
-      </c>
-      <c r="D14" s="13">
-        <v>1.52385183272547</v>
-      </c>
-      <c r="E14" s="13">
-        <v>1.41449419584761</v>
-      </c>
-      <c r="F14" s="14">
-        <v>1.30515604992627</v>
-      </c>
-      <c r="G14" s="12">
-        <v>1.88318956466904</v>
-      </c>
-      <c r="H14" s="13">
-        <v>1.7076448816340799</v>
-      </c>
-      <c r="I14" s="15">
-        <v>1.5489753422189001</v>
-      </c>
-      <c r="J14" s="11">
-        <v>1.4115185490528199</v>
+      <c r="C14" s="23">
+        <v>1.63493330920942</v>
+      </c>
+      <c r="D14" s="24">
+        <v>1.5249480720057</v>
+      </c>
+      <c r="E14" s="24">
+        <v>1.41558231001086</v>
+      </c>
+      <c r="F14" s="25">
+        <v>1.3062445376015399</v>
+      </c>
+      <c r="G14" s="22">
+        <v>1.8850823267521499</v>
+      </c>
+      <c r="H14" s="24">
+        <v>1.70951327092703</v>
+      </c>
+      <c r="I14" s="24">
+        <v>1.5498599703229801</v>
+      </c>
+      <c r="J14" s="25">
+        <v>1.4126806078093499</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
+      <c r="A15" s="7">
         <v>0.15</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="8">
         <v>4.6209812037329696</v>
       </c>
-      <c r="C15" s="18">
-        <v>2.0036440472798001</v>
-      </c>
-      <c r="D15" s="19">
-        <v>1.83134837447231</v>
-      </c>
-      <c r="E15" s="19">
-        <v>1.6588657235995601</v>
-      </c>
-      <c r="F15" s="20">
-        <v>1.4859600316274799</v>
-      </c>
-      <c r="G15" s="18">
-        <v>2.5107248454564299</v>
-      </c>
-      <c r="H15" s="19">
-        <v>2.1706771311107498</v>
-      </c>
-      <c r="I15" s="21">
-        <v>1.8781226644559099</v>
-      </c>
-      <c r="J15" s="17">
-        <v>1.63827951121272</v>
+      <c r="C15" s="23">
+        <v>2.0053430365752098</v>
+      </c>
+      <c r="D15" s="24">
+        <v>1.83307339190802</v>
+      </c>
+      <c r="E15" s="24">
+        <v>1.6605840772823</v>
+      </c>
+      <c r="F15" s="25">
+        <v>1.4876806423473601</v>
+      </c>
+      <c r="G15" s="22">
+        <v>2.5144909648920302</v>
+      </c>
+      <c r="H15" s="24">
+        <v>2.1741613852848101</v>
+      </c>
+      <c r="I15" s="24">
+        <v>1.87982176076535</v>
+      </c>
+      <c r="J15" s="25">
+        <v>1.64027317370503</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="16">
+      <c r="A16" s="7">
         <v>0.2</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="8">
         <v>3.4657359027997301</v>
       </c>
-      <c r="C16" s="18">
-        <v>2.3974766812193602</v>
-      </c>
-      <c r="D16" s="19">
-        <v>2.15763167725135</v>
-      </c>
-      <c r="E16" s="19">
-        <v>1.9168171271588901</v>
-      </c>
-      <c r="F16" s="20">
-        <v>1.6749473249504501</v>
-      </c>
-      <c r="G16" s="18">
-        <v>3.29320792679589</v>
-      </c>
-      <c r="H16" s="19">
-        <v>2.71777782255612</v>
-      </c>
-      <c r="I16" s="21">
-        <v>2.24629143901798</v>
-      </c>
-      <c r="J16" s="17">
-        <v>1.88002126192431</v>
+      <c r="C16" s="23">
+        <v>2.39983048131606</v>
+      </c>
+      <c r="D16" s="24">
+        <v>2.1600356692164699</v>
+      </c>
+      <c r="E16" s="24">
+        <v>1.9192187017742199</v>
+      </c>
+      <c r="F16" s="25">
+        <v>1.67735308043784</v>
+      </c>
+      <c r="G16" s="22">
+        <v>3.2997495515161699</v>
+      </c>
+      <c r="H16" s="24">
+        <v>2.7234615697895399</v>
+      </c>
+      <c r="I16" s="24">
+        <v>2.2490980447704398</v>
+      </c>
+      <c r="J16" s="25">
+        <v>1.8829993980433199</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="16">
+      <c r="A17" s="7">
         <v>0.25</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="8">
         <v>2.7725887222397798</v>
       </c>
-      <c r="C17" s="18">
-        <v>2.8135612466250599</v>
-      </c>
-      <c r="D17" s="19">
-        <v>2.5015686508056199</v>
-      </c>
-      <c r="E17" s="19">
-        <v>2.18769196507519</v>
-      </c>
-      <c r="F17" s="20">
-        <v>1.8718543005702</v>
-      </c>
-      <c r="G17" s="18">
-        <v>4.2571643436741704</v>
-      </c>
-      <c r="H17" s="19">
-        <v>3.3578657045712399</v>
-      </c>
-      <c r="I17" s="21">
-        <v>2.6553657109814002</v>
-      </c>
-      <c r="J17" s="17">
-        <v>2.1371454056767099</v>
+      <c r="C17" s="23">
+        <v>2.8166091096647499</v>
+      </c>
+      <c r="D17" s="24">
+        <v>2.5046961052131</v>
+      </c>
+      <c r="E17" s="24">
+        <v>2.1908257664972299</v>
+      </c>
+      <c r="F17" s="25">
+        <v>1.87499445742846</v>
+      </c>
+      <c r="G17" s="22">
+        <v>4.26764949471786</v>
+      </c>
+      <c r="H17" s="24">
+        <v>3.3664411152474698</v>
+      </c>
+      <c r="I17" s="24">
+        <v>2.6596066021682598</v>
+      </c>
+      <c r="J17" s="25">
+        <v>2.1412582149027699</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="22">
+      <c r="A18" s="9">
         <v>0.3</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="10">
         <v>2.3104906018664799</v>
       </c>
-      <c r="C18" s="24">
-        <v>3.25054887144467</v>
-      </c>
-      <c r="D18" s="25">
-        <v>2.86221416963788</v>
-      </c>
-      <c r="E18" s="25">
-        <v>2.4709067260473301</v>
-      </c>
-      <c r="F18" s="26">
-        <v>2.07643064486449</v>
-      </c>
-      <c r="G18" s="24">
-        <v>5.4318954085080096</v>
-      </c>
-      <c r="H18" s="25">
-        <v>4.1002261777418703</v>
-      </c>
-      <c r="I18" s="27">
-        <v>3.1072051921509898</v>
-      </c>
-      <c r="J18" s="23">
-        <v>2.4099722881572898</v>
+      <c r="C18" s="23">
+        <v>3.2543254066865099</v>
+      </c>
+      <c r="D18" s="24">
+        <v>2.8661053409439701</v>
+      </c>
+      <c r="E18" s="24">
+        <v>2.4748186204518201</v>
+      </c>
+      <c r="F18" s="25">
+        <v>2.0803511663873002</v>
+      </c>
+      <c r="G18" s="22">
+        <v>5.44780521143797</v>
+      </c>
+      <c r="H18" s="24">
+        <v>4.1125033124849502</v>
+      </c>
+      <c r="I18" s="24">
+        <v>3.11324031594833</v>
+      </c>
+      <c r="J18" s="25">
+        <v>2.4153694477864098</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="3">
-        <v>6.2038457846732999</v>
-      </c>
-      <c r="D19" s="4">
-        <v>5.36871234446419</v>
-      </c>
-      <c r="E19" s="4">
-        <v>4.3989469801442196</v>
-      </c>
-      <c r="F19" s="7">
-        <v>3.3868438663914202</v>
-      </c>
-      <c r="G19" s="3">
-        <v>6.8057307581915802</v>
-      </c>
-      <c r="H19" s="4">
-        <v>5.8401803322494503</v>
-      </c>
-      <c r="I19" s="9">
-        <v>4.7756263802154599</v>
-      </c>
-      <c r="J19" s="6">
-        <v>3.8042262548830101</v>
+      <c r="B19" s="21"/>
+      <c r="C19" s="26">
+        <v>6.2115346326912801</v>
+      </c>
+      <c r="D19" s="27">
+        <v>5.3781394856754599</v>
+      </c>
+      <c r="E19" s="27">
+        <v>4.4088575347563603</v>
+      </c>
+      <c r="F19" s="28">
+        <v>3.3970223714276702</v>
+      </c>
+      <c r="G19" s="29">
+        <v>6.8160399417984401</v>
+      </c>
+      <c r="H19" s="27">
+        <v>5.8516363929559798</v>
+      </c>
+      <c r="I19" s="27">
+        <v>4.7973983744078801</v>
+      </c>
+      <c r="J19" s="28">
+        <v>3.81243411882136</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="G2:J2"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C11:F11"/>
@@ -1575,6 +1525,13 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="G2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>